<commit_message>
finished gropin growth models
Signed-off-by: Ruediger <dr.marcel.fuhrmann@gmail.com>
</commit_message>
<xml_diff>
--- a/gropin/schema/metadataschema1033.xlsx
+++ b/gropin/schema/metadataschema1033.xlsx
@@ -632,7 +632,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Gropin growth model for Saccharomyces cerevisiae in/on Wines, beverages, fruit concentrates, preserves (gropin ID: 1033 )</t>
+          <t>Gropin secondary growth model for Saccharomyces cerevisiae in/on Wines, beverages, fruit concentrates, preserves (gropin ID: 1033 )</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>QRA model</t>
+          <t>Predictive</t>
         </is>
       </c>
     </row>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>seq(0.1001,49.95004995005,length.out=21)</t>
+          <t>seq(0.1001,49.95004995005,length.out=10)</t>
         </is>
       </c>
     </row>
@@ -5346,7 +5346,7 @@
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>seq(0,11.988011988012,length.out=21)</t>
+          <t>seq(0,11.988011988012,length.out=10)</t>
         </is>
       </c>
     </row>
@@ -5403,7 +5403,7 @@
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>seq(2.5025,7.99200799200799,length.out=21)</t>
+          <t>seq(2.5025,7.99200799200799,length.out=10)</t>
         </is>
       </c>
     </row>

</xml_diff>